<commit_message>
Screenshots and new code
</commit_message>
<xml_diff>
--- a/Recursos.xlsx
+++ b/Recursos.xlsx
@@ -7,8 +7,8 @@
     <workbookView xWindow="240" yWindow="75" windowWidth="20115" windowHeight="8505"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Recursos Naturales" sheetId="1" r:id="rId1"/>
+    <sheet name="Productos" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="125725"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="255" uniqueCount="118">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="255" uniqueCount="117">
   <si>
     <t>Recursos Naturales</t>
   </si>
@@ -34,9 +34,6 @@
   </si>
   <si>
     <t>Granito</t>
-  </si>
-  <si>
-    <t>Contruccion</t>
   </si>
   <si>
     <t>Construccion</t>
@@ -858,8 +855,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:Q83"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A46" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="O83" sqref="O83:Q83"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="Q4" sqref="Q4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -930,12 +927,12 @@
       <c r="D8" s="8"/>
       <c r="E8" s="8"/>
       <c r="G8" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="H8" s="1"/>
       <c r="I8" s="1"/>
       <c r="K8" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="L8" s="1"/>
       <c r="M8" s="1"/>
@@ -945,17 +942,17 @@
         <v>2</v>
       </c>
       <c r="C9" s="8" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D9" s="8"/>
       <c r="E9" s="8"/>
       <c r="G9" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="H9" s="1"/>
       <c r="I9" s="1"/>
       <c r="K9" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="L9" s="1"/>
       <c r="M9" s="1"/>
@@ -965,7 +962,7 @@
         <v>3</v>
       </c>
       <c r="C10" s="8" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D10" s="8"/>
       <c r="E10" s="8"/>
@@ -975,7 +972,7 @@
       <c r="H10" s="11"/>
       <c r="I10" s="11"/>
       <c r="K10" s="11" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="L10" s="11"/>
       <c r="M10" s="11"/>
@@ -985,17 +982,17 @@
         <v>4</v>
       </c>
       <c r="C11" s="8" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D11" s="8"/>
       <c r="E11" s="8"/>
       <c r="G11" s="11" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="H11" s="11"/>
       <c r="I11" s="11"/>
       <c r="K11" s="11" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="L11" s="11"/>
       <c r="M11" s="11"/>
@@ -1005,17 +1002,17 @@
         <v>5</v>
       </c>
       <c r="C12" s="8" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D12" s="8"/>
       <c r="E12" s="8"/>
       <c r="G12" s="11" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="H12" s="11"/>
       <c r="I12" s="11"/>
       <c r="K12" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="L12" s="1"/>
       <c r="M12" s="1"/>
@@ -1025,17 +1022,17 @@
         <v>6</v>
       </c>
       <c r="C13" s="8" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D13" s="8"/>
       <c r="E13" s="8"/>
       <c r="G13" s="11" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="H13" s="11"/>
       <c r="I13" s="11"/>
       <c r="K13" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="L13" s="1"/>
       <c r="M13" s="1"/>
@@ -1045,17 +1042,17 @@
         <v>7</v>
       </c>
       <c r="C14" s="8" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D14" s="8"/>
       <c r="E14" s="8"/>
       <c r="G14" s="11" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="H14" s="11"/>
       <c r="I14" s="11"/>
       <c r="K14" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="L14" s="1"/>
       <c r="M14" s="1"/>
@@ -1065,17 +1062,17 @@
         <v>8</v>
       </c>
       <c r="C15" s="8" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D15" s="8"/>
       <c r="E15" s="8"/>
       <c r="G15" s="11" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="H15" s="11"/>
       <c r="I15" s="11"/>
       <c r="K15" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="L15" s="1"/>
       <c r="M15" s="1"/>
@@ -1085,17 +1082,17 @@
         <v>9</v>
       </c>
       <c r="C16" s="8" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D16" s="8"/>
       <c r="E16" s="8"/>
       <c r="G16" s="11" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="H16" s="11"/>
       <c r="I16" s="11"/>
       <c r="K16" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="L16" s="1"/>
       <c r="M16" s="1"/>
@@ -1105,17 +1102,17 @@
         <v>10</v>
       </c>
       <c r="C17" s="8" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D17" s="8"/>
       <c r="E17" s="8"/>
       <c r="G17" s="11" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="H17" s="11"/>
       <c r="I17" s="11"/>
       <c r="K17" s="11" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="L17" s="11"/>
       <c r="M17" s="11"/>
@@ -1125,17 +1122,17 @@
         <v>11</v>
       </c>
       <c r="C18" s="8" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D18" s="8"/>
       <c r="E18" s="8"/>
       <c r="G18" s="11" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="H18" s="11"/>
       <c r="I18" s="11"/>
       <c r="K18" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="L18" s="1"/>
       <c r="M18" s="1"/>
@@ -1145,17 +1142,17 @@
         <v>12</v>
       </c>
       <c r="C19" s="8" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D19" s="8"/>
       <c r="E19" s="8"/>
       <c r="G19" s="11" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="H19" s="11"/>
       <c r="I19" s="11"/>
       <c r="K19" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="L19" s="1"/>
       <c r="M19" s="1"/>
@@ -1165,17 +1162,17 @@
         <v>13</v>
       </c>
       <c r="C20" s="8" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D20" s="8"/>
       <c r="E20" s="8"/>
       <c r="G20" s="11" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="H20" s="11"/>
       <c r="I20" s="11"/>
       <c r="K20" s="11" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="L20" s="11"/>
       <c r="M20" s="11"/>
@@ -1185,17 +1182,17 @@
         <v>14</v>
       </c>
       <c r="C21" s="8" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D21" s="8"/>
       <c r="E21" s="8"/>
       <c r="G21" s="11" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="H21" s="11"/>
       <c r="I21" s="11"/>
       <c r="K21" s="11" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="L21" s="11"/>
       <c r="M21" s="11"/>
@@ -1206,16 +1203,16 @@
       </c>
       <c r="C22" s="9"/>
       <c r="D22" s="9" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="E22" s="9"/>
       <c r="G22" s="11" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="H22" s="11"/>
       <c r="I22" s="11"/>
       <c r="K22" s="11" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="L22" s="11"/>
       <c r="M22" s="11"/>
@@ -1225,17 +1222,17 @@
         <v>16</v>
       </c>
       <c r="C23" s="8" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="D23" s="8"/>
       <c r="E23" s="8"/>
       <c r="G23" s="11" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="H23" s="11"/>
       <c r="I23" s="11"/>
       <c r="K23" s="11" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="L23" s="11"/>
       <c r="M23" s="11"/>
@@ -1248,17 +1245,17 @@
         <v>17</v>
       </c>
       <c r="C24" s="8" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="D24" s="8"/>
       <c r="E24" s="8"/>
       <c r="G24" s="11" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="H24" s="11"/>
       <c r="I24" s="11"/>
       <c r="K24" s="11" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="L24" s="11"/>
       <c r="M24" s="11"/>
@@ -1289,12 +1286,12 @@
       <c r="H26" s="3"/>
       <c r="I26" s="3"/>
       <c r="K26" s="3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="L26" s="3"/>
       <c r="M26" s="3"/>
       <c r="O26" s="3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="P26" s="3"/>
       <c r="Q26" s="3"/>
@@ -1315,7 +1312,7 @@
     </row>
     <row r="28" spans="1:17">
       <c r="C28" s="14" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D28" s="14"/>
       <c r="E28" s="14"/>
@@ -1348,22 +1345,22 @@
         <v>18</v>
       </c>
       <c r="C30" s="13" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D30" s="12"/>
       <c r="E30" s="12"/>
       <c r="G30" s="6" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="H30" s="6"/>
       <c r="I30" s="6"/>
       <c r="K30" s="6" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="L30" s="6"/>
       <c r="M30" s="6"/>
       <c r="O30" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="P30" s="1"/>
       <c r="Q30" s="1"/>
@@ -1373,22 +1370,22 @@
         <v>19</v>
       </c>
       <c r="C31" s="13" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D31" s="12"/>
       <c r="E31" s="12"/>
       <c r="G31" s="6" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="H31" s="6"/>
       <c r="I31" s="6"/>
       <c r="K31" s="6" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="L31" s="6"/>
       <c r="M31" s="6"/>
       <c r="O31" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="P31" s="1"/>
       <c r="Q31" s="1"/>
@@ -1398,22 +1395,22 @@
         <v>20</v>
       </c>
       <c r="C32" s="13" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D32" s="12"/>
       <c r="E32" s="12"/>
       <c r="G32" s="6" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="H32" s="6"/>
       <c r="I32" s="6"/>
       <c r="K32" s="6" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="L32" s="6"/>
       <c r="M32" s="6"/>
       <c r="O32" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="P32" s="1"/>
       <c r="Q32" s="1"/>
@@ -1423,22 +1420,22 @@
         <v>21</v>
       </c>
       <c r="C33" s="13" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D33" s="12"/>
       <c r="E33" s="12"/>
       <c r="G33" s="6" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="H33" s="6"/>
       <c r="I33" s="6"/>
       <c r="K33" s="6" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="L33" s="6"/>
       <c r="M33" s="6"/>
       <c r="O33" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="P33" s="1"/>
       <c r="Q33" s="1"/>
@@ -1448,22 +1445,22 @@
         <v>22</v>
       </c>
       <c r="C34" s="13" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D34" s="12"/>
       <c r="E34" s="12"/>
       <c r="G34" s="6" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="H34" s="6"/>
       <c r="I34" s="6"/>
       <c r="K34" s="6" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="L34" s="6"/>
       <c r="M34" s="6"/>
       <c r="O34" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="P34" s="1"/>
       <c r="Q34" s="1"/>
@@ -1473,22 +1470,22 @@
         <v>23</v>
       </c>
       <c r="C35" s="13" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D35" s="12"/>
       <c r="E35" s="12"/>
       <c r="G35" s="6" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="H35" s="6"/>
       <c r="I35" s="6"/>
       <c r="K35" s="6" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="L35" s="6"/>
       <c r="M35" s="6"/>
       <c r="O35" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="P35" s="1"/>
       <c r="Q35" s="1"/>
@@ -1498,22 +1495,22 @@
         <v>24</v>
       </c>
       <c r="C36" s="13" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D36" s="12"/>
       <c r="E36" s="12"/>
       <c r="G36" s="6" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="H36" s="6"/>
       <c r="I36" s="6"/>
       <c r="K36" s="6" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="L36" s="6"/>
       <c r="M36" s="6"/>
       <c r="O36" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="P36" s="1"/>
       <c r="Q36" s="1"/>
@@ -1523,22 +1520,22 @@
         <v>25</v>
       </c>
       <c r="C37" s="13" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D37" s="12"/>
       <c r="E37" s="12"/>
       <c r="G37" s="6" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="H37" s="6"/>
       <c r="I37" s="6"/>
       <c r="K37" s="6" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="L37" s="6"/>
       <c r="M37" s="6"/>
       <c r="O37" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="P37" s="1"/>
       <c r="Q37" s="1"/>
@@ -1548,22 +1545,22 @@
         <v>26</v>
       </c>
       <c r="C38" s="13" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D38" s="12"/>
       <c r="E38" s="12"/>
       <c r="G38" s="6" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="H38" s="6"/>
       <c r="I38" s="6"/>
       <c r="K38" s="6" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="L38" s="6"/>
       <c r="M38" s="6"/>
       <c r="O38" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="P38" s="1"/>
       <c r="Q38" s="1"/>
@@ -1573,22 +1570,22 @@
         <v>27</v>
       </c>
       <c r="C39" s="13" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D39" s="12"/>
       <c r="E39" s="12"/>
       <c r="G39" s="6" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="H39" s="6"/>
       <c r="I39" s="6"/>
       <c r="K39" s="6" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="L39" s="6"/>
       <c r="M39" s="6"/>
       <c r="O39" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="P39" s="1"/>
       <c r="Q39" s="1"/>
@@ -1598,22 +1595,22 @@
         <v>28</v>
       </c>
       <c r="C40" s="13" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D40" s="12"/>
       <c r="E40" s="12"/>
       <c r="G40" s="6" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="H40" s="6"/>
       <c r="I40" s="6"/>
       <c r="K40" s="11" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="L40" s="11"/>
       <c r="M40" s="11"/>
       <c r="O40" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="P40" s="1"/>
       <c r="Q40" s="1"/>
@@ -1623,22 +1620,22 @@
         <v>29</v>
       </c>
       <c r="C41" s="13" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D41" s="12"/>
       <c r="E41" s="12"/>
       <c r="G41" s="6" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="H41" s="6"/>
       <c r="I41" s="6"/>
       <c r="K41" s="11" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="L41" s="11"/>
       <c r="M41" s="11"/>
       <c r="O41" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="P41" s="1"/>
       <c r="Q41" s="1"/>
@@ -1648,22 +1645,22 @@
         <v>30</v>
       </c>
       <c r="C42" s="13" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D42" s="12"/>
       <c r="E42" s="12"/>
       <c r="G42" s="6" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="H42" s="6"/>
       <c r="I42" s="6"/>
       <c r="K42" s="6" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="L42" s="6"/>
       <c r="M42" s="6"/>
       <c r="O42" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="P42" s="1"/>
       <c r="Q42" s="1"/>
@@ -1673,22 +1670,22 @@
         <v>31</v>
       </c>
       <c r="C43" s="13" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D43" s="12"/>
       <c r="E43" s="12"/>
       <c r="G43" s="6" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="H43" s="6"/>
       <c r="I43" s="6"/>
       <c r="K43" s="6" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="L43" s="6"/>
       <c r="M43" s="6"/>
       <c r="O43" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="P43" s="1"/>
       <c r="Q43" s="1"/>
@@ -1698,22 +1695,22 @@
         <v>32</v>
       </c>
       <c r="C44" s="13" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D44" s="12"/>
       <c r="E44" s="12"/>
       <c r="G44" s="6" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="H44" s="6"/>
       <c r="I44" s="6"/>
       <c r="K44" s="6" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="L44" s="6"/>
       <c r="M44" s="6"/>
       <c r="O44" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="P44" s="1"/>
       <c r="Q44" s="1"/>
@@ -1723,22 +1720,22 @@
         <v>33</v>
       </c>
       <c r="C45" s="13" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D45" s="12"/>
       <c r="E45" s="12"/>
       <c r="G45" s="6" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="H45" s="6"/>
       <c r="I45" s="6"/>
       <c r="K45" s="6" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="L45" s="6"/>
       <c r="M45" s="6"/>
       <c r="O45" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="P45" s="1"/>
       <c r="Q45" s="1"/>
@@ -1748,22 +1745,22 @@
         <v>34</v>
       </c>
       <c r="C46" s="13" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D46" s="12"/>
       <c r="E46" s="12"/>
       <c r="G46" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="H46" s="1"/>
       <c r="I46" s="1"/>
       <c r="K46" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="L46" s="1"/>
       <c r="M46" s="1"/>
       <c r="O46" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="P46" s="1"/>
       <c r="Q46" s="1"/>
@@ -1773,22 +1770,22 @@
         <v>35</v>
       </c>
       <c r="C47" s="13" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D47" s="12"/>
       <c r="E47" s="12"/>
       <c r="G47" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="H47" s="1"/>
       <c r="I47" s="1"/>
       <c r="K47" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="L47" s="1"/>
       <c r="M47" s="1"/>
       <c r="O47" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="P47" s="1"/>
       <c r="Q47" s="1"/>
@@ -1798,22 +1795,22 @@
         <v>36</v>
       </c>
       <c r="C48" s="13" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D48" s="12"/>
       <c r="E48" s="12"/>
       <c r="G48" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="H48" s="1"/>
       <c r="I48" s="1"/>
       <c r="K48" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="L48" s="1"/>
       <c r="M48" s="1"/>
       <c r="O48" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="P48" s="1"/>
       <c r="Q48" s="1"/>
@@ -1823,22 +1820,22 @@
         <v>37</v>
       </c>
       <c r="C49" s="13" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D49" s="12"/>
       <c r="E49" s="12"/>
       <c r="G49" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="H49" s="1"/>
       <c r="I49" s="1"/>
       <c r="K49" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="L49" s="1"/>
       <c r="M49" s="1"/>
       <c r="O49" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="P49" s="1"/>
       <c r="Q49" s="1"/>
@@ -1848,22 +1845,22 @@
         <v>38</v>
       </c>
       <c r="C50" s="13" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D50" s="12"/>
       <c r="E50" s="12"/>
       <c r="G50" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="H50" s="1"/>
       <c r="I50" s="1"/>
       <c r="K50" s="11" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="L50" s="11"/>
       <c r="M50" s="11"/>
       <c r="O50" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="P50" s="1"/>
       <c r="Q50" s="1"/>
@@ -1873,22 +1870,22 @@
         <v>39</v>
       </c>
       <c r="C51" s="13" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D51" s="12"/>
       <c r="E51" s="12"/>
       <c r="G51" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="H51" s="1"/>
       <c r="I51" s="1"/>
       <c r="K51" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="L51" s="1"/>
       <c r="M51" s="1"/>
       <c r="O51" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="P51" s="1"/>
       <c r="Q51" s="1"/>
@@ -1898,29 +1895,29 @@
         <v>40</v>
       </c>
       <c r="C52" s="13" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D52" s="12"/>
       <c r="E52" s="12"/>
       <c r="G52" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="H52" s="1"/>
       <c r="I52" s="1"/>
       <c r="K52" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="L52" s="1"/>
       <c r="M52" s="1"/>
       <c r="O52" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="P52" s="1"/>
       <c r="Q52" s="1"/>
     </row>
     <row r="53" spans="1:17">
       <c r="C53" s="4" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D53" s="4"/>
       <c r="E53" s="4"/>
@@ -1946,12 +1943,12 @@
       <c r="H54" s="3"/>
       <c r="I54" s="3"/>
       <c r="K54" s="3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="L54" s="3"/>
       <c r="M54" s="3"/>
       <c r="O54" s="3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="P54" s="3"/>
       <c r="Q54" s="3"/>
@@ -1972,7 +1969,7 @@
     </row>
     <row r="56" spans="1:17">
       <c r="C56" s="18" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D56" s="18"/>
       <c r="E56" s="18"/>
@@ -2005,22 +2002,22 @@
         <v>41</v>
       </c>
       <c r="C58" s="17" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D58" s="16"/>
       <c r="E58" s="16"/>
       <c r="G58" s="6" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="H58" s="6"/>
       <c r="I58" s="6"/>
       <c r="K58" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="L58" s="1"/>
       <c r="M58" s="1"/>
       <c r="O58" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="P58" s="1"/>
       <c r="Q58" s="1"/>
@@ -2030,22 +2027,22 @@
         <v>42</v>
       </c>
       <c r="C59" s="17" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D59" s="16"/>
       <c r="E59" s="16"/>
       <c r="G59" s="6" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="H59" s="6"/>
       <c r="I59" s="6"/>
       <c r="K59" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="L59" s="1"/>
       <c r="M59" s="1"/>
       <c r="O59" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="P59" s="1"/>
       <c r="Q59" s="1"/>
@@ -2055,22 +2052,22 @@
         <v>43</v>
       </c>
       <c r="C60" s="17" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D60" s="16"/>
       <c r="E60" s="16"/>
       <c r="G60" s="6" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="H60" s="6"/>
       <c r="I60" s="6"/>
       <c r="K60" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="L60" s="1"/>
       <c r="M60" s="1"/>
       <c r="O60" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="P60" s="1"/>
       <c r="Q60" s="1"/>
@@ -2080,22 +2077,22 @@
         <v>44</v>
       </c>
       <c r="C61" s="17" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D61" s="16"/>
       <c r="E61" s="16"/>
       <c r="G61" s="6" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="H61" s="6"/>
       <c r="I61" s="6"/>
       <c r="K61" s="11" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="L61" s="11"/>
       <c r="M61" s="11"/>
       <c r="O61" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="P61" s="1"/>
       <c r="Q61" s="1"/>
@@ -2105,22 +2102,22 @@
         <v>45</v>
       </c>
       <c r="C62" s="17" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D62" s="16"/>
       <c r="E62" s="16"/>
       <c r="G62" s="6" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="H62" s="6"/>
       <c r="I62" s="6"/>
       <c r="K62" s="11" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="L62" s="11"/>
       <c r="M62" s="11"/>
       <c r="O62" s="11" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="P62" s="11"/>
       <c r="Q62" s="11"/>
@@ -2130,22 +2127,22 @@
         <v>46</v>
       </c>
       <c r="C63" s="17" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D63" s="16"/>
       <c r="E63" s="16"/>
       <c r="G63" s="6" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="H63" s="6"/>
       <c r="I63" s="6"/>
       <c r="K63" s="11" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="L63" s="11"/>
       <c r="M63" s="11"/>
       <c r="O63" s="11" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="P63" s="11"/>
       <c r="Q63" s="11"/>
@@ -2155,22 +2152,22 @@
         <v>47</v>
       </c>
       <c r="C64" s="17" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D64" s="16"/>
       <c r="E64" s="16"/>
       <c r="G64" s="6" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="H64" s="6"/>
       <c r="I64" s="6"/>
       <c r="K64" s="11" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="L64" s="11"/>
       <c r="M64" s="11"/>
       <c r="O64" s="11" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="P64" s="11"/>
       <c r="Q64" s="11"/>
@@ -2180,22 +2177,22 @@
         <v>48</v>
       </c>
       <c r="C65" s="17" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D65" s="16"/>
       <c r="E65" s="16"/>
       <c r="G65" s="6" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="H65" s="6"/>
       <c r="I65" s="6"/>
       <c r="K65" s="11" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="L65" s="11"/>
       <c r="M65" s="11"/>
       <c r="O65" s="11" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="P65" s="11"/>
       <c r="Q65" s="11"/>
@@ -2205,22 +2202,22 @@
         <v>49</v>
       </c>
       <c r="C66" s="17" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D66" s="16"/>
       <c r="E66" s="16"/>
       <c r="G66" s="6" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="H66" s="6"/>
       <c r="I66" s="6"/>
       <c r="K66" s="11" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="L66" s="11"/>
       <c r="M66" s="11"/>
       <c r="O66" s="11" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="P66" s="11"/>
       <c r="Q66" s="11"/>
@@ -2230,22 +2227,22 @@
         <v>50</v>
       </c>
       <c r="C67" s="17" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D67" s="16"/>
       <c r="E67" s="16"/>
       <c r="G67" s="6" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="H67" s="6"/>
       <c r="I67" s="6"/>
       <c r="K67" s="11" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="L67" s="11"/>
       <c r="M67" s="11"/>
       <c r="O67" s="11" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="P67" s="11"/>
       <c r="Q67" s="11"/>
@@ -2255,22 +2252,22 @@
         <v>51</v>
       </c>
       <c r="C68" s="17" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D68" s="16"/>
       <c r="E68" s="16"/>
       <c r="G68" s="6" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="H68" s="6"/>
       <c r="I68" s="6"/>
       <c r="K68" s="11" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="L68" s="11"/>
       <c r="M68" s="11"/>
       <c r="O68" s="11" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="P68" s="11"/>
       <c r="Q68" s="11"/>
@@ -2280,22 +2277,22 @@
         <v>52</v>
       </c>
       <c r="C69" s="17" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D69" s="16"/>
       <c r="E69" s="16"/>
       <c r="G69" s="6" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="H69" s="6"/>
       <c r="I69" s="6"/>
       <c r="K69" s="11" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="L69" s="11"/>
       <c r="M69" s="11"/>
       <c r="O69" s="11" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="P69" s="11"/>
       <c r="Q69" s="11"/>
@@ -2305,22 +2302,22 @@
         <v>53</v>
       </c>
       <c r="C70" s="17" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D70" s="16"/>
       <c r="E70" s="16"/>
       <c r="G70" s="6" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="H70" s="6"/>
       <c r="I70" s="6"/>
       <c r="K70" s="11" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="L70" s="11"/>
       <c r="M70" s="11"/>
       <c r="O70" s="11" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="P70" s="11"/>
       <c r="Q70" s="11"/>
@@ -2330,22 +2327,22 @@
         <v>54</v>
       </c>
       <c r="C71" s="17" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D71" s="16"/>
       <c r="E71" s="16"/>
       <c r="G71" s="6" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="H71" s="6"/>
       <c r="I71" s="6"/>
       <c r="K71" s="11" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="L71" s="11"/>
       <c r="M71" s="11"/>
       <c r="O71" s="11" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="P71" s="11"/>
       <c r="Q71" s="11"/>
@@ -2355,22 +2352,22 @@
         <v>55</v>
       </c>
       <c r="C72" s="17" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D72" s="16"/>
       <c r="E72" s="16"/>
       <c r="G72" s="6" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="H72" s="6"/>
       <c r="I72" s="6"/>
       <c r="K72" s="11" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="L72" s="11"/>
       <c r="M72" s="11"/>
       <c r="O72" s="11" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="P72" s="11"/>
       <c r="Q72" s="11"/>
@@ -2380,22 +2377,22 @@
         <v>56</v>
       </c>
       <c r="C73" s="17" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D73" s="16"/>
       <c r="E73" s="16"/>
       <c r="G73" s="6" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="H73" s="6"/>
       <c r="I73" s="6"/>
       <c r="K73" s="11" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="L73" s="11"/>
       <c r="M73" s="11"/>
       <c r="O73" s="11" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="P73" s="11"/>
       <c r="Q73" s="11"/>
@@ -2405,22 +2402,22 @@
         <v>57</v>
       </c>
       <c r="C74" s="17" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="D74" s="16"/>
       <c r="E74" s="16"/>
       <c r="G74" s="6" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="H74" s="6"/>
       <c r="I74" s="6"/>
       <c r="K74" s="11" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="L74" s="11"/>
       <c r="M74" s="11"/>
       <c r="O74" s="11" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="P74" s="11"/>
       <c r="Q74" s="11"/>
@@ -2430,22 +2427,22 @@
         <v>58</v>
       </c>
       <c r="C75" s="17" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D75" s="16"/>
       <c r="E75" s="16"/>
       <c r="G75" s="6" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="H75" s="6"/>
       <c r="I75" s="6"/>
       <c r="K75" s="11" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="L75" s="11"/>
       <c r="M75" s="11"/>
       <c r="O75" s="11" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="P75" s="11"/>
       <c r="Q75" s="11"/>
@@ -2455,22 +2452,22 @@
         <v>59</v>
       </c>
       <c r="C76" s="17" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D76" s="16"/>
       <c r="E76" s="16"/>
       <c r="G76" s="6" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="H76" s="6"/>
       <c r="I76" s="6"/>
       <c r="K76" s="11" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="L76" s="11"/>
       <c r="M76" s="11"/>
       <c r="O76" s="11" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="P76" s="11"/>
       <c r="Q76" s="11"/>
@@ -2480,22 +2477,22 @@
         <v>60</v>
       </c>
       <c r="C77" s="17" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D77" s="16"/>
       <c r="E77" s="16"/>
       <c r="G77" s="6" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="H77" s="6"/>
       <c r="I77" s="6"/>
       <c r="K77" s="11" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="L77" s="11"/>
       <c r="M77" s="11"/>
       <c r="O77" s="11" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="P77" s="11"/>
       <c r="Q77" s="11"/>
@@ -2505,22 +2502,22 @@
         <v>61</v>
       </c>
       <c r="C78" s="17" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="D78" s="16"/>
       <c r="E78" s="16"/>
       <c r="G78" s="6" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="H78" s="6"/>
       <c r="I78" s="6"/>
       <c r="K78" s="11" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="L78" s="11"/>
       <c r="M78" s="11"/>
       <c r="O78" s="11" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="P78" s="11"/>
       <c r="Q78" s="11"/>
@@ -2530,22 +2527,22 @@
         <v>62</v>
       </c>
       <c r="C79" s="17" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="D79" s="16"/>
       <c r="E79" s="16"/>
       <c r="G79" s="6" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="H79" s="6"/>
       <c r="I79" s="6"/>
       <c r="K79" s="11" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="L79" s="11"/>
       <c r="M79" s="11"/>
       <c r="O79" s="11" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="P79" s="11"/>
       <c r="Q79" s="11"/>
@@ -2555,22 +2552,22 @@
         <v>63</v>
       </c>
       <c r="C80" s="17" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="D80" s="16"/>
       <c r="E80" s="16"/>
       <c r="G80" s="6" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="H80" s="6"/>
       <c r="I80" s="6"/>
       <c r="K80" s="11" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="L80" s="11"/>
       <c r="M80" s="11"/>
       <c r="O80" s="11" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="P80" s="11"/>
       <c r="Q80" s="11"/>
@@ -2580,22 +2577,22 @@
         <v>64</v>
       </c>
       <c r="C81" s="17" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="D81" s="16"/>
       <c r="E81" s="16"/>
       <c r="G81" s="6" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="H81" s="6"/>
       <c r="I81" s="6"/>
       <c r="K81" s="11" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="L81" s="11"/>
       <c r="M81" s="11"/>
       <c r="O81" s="11" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="P81" s="11"/>
       <c r="Q81" s="11"/>

</xml_diff>